<commit_message>
changemanagement + scrumboard update
</commit_message>
<xml_diff>
--- a/MUH PRE/SCRUMBOARD SmartGastro.xlsx
+++ b/MUH PRE/SCRUMBOARD SmartGastro.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Misa\Desktop\SmartGastro MUH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Misa\Desktop\SYP_SmartGastro\MUH PRE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA55723E-35BB-44A5-AE44-B7577CB0B67B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C8575C-D3D2-4834-A429-37AF3E0F612C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{13228F70-B0DF-44E9-9012-5AA6642C623D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>SmartGastro</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Use Case Diagramm - LOT</t>
   </si>
   <si>
-    <t>GUI für die Android App</t>
-  </si>
-  <si>
     <t>MenuItem Getränke</t>
   </si>
   <si>
@@ -113,12 +110,6 @@
     <t>Prozedur Gesamtpreis</t>
   </si>
   <si>
-    <t>Mockups Android App</t>
-  </si>
-  <si>
-    <t>Mockups HTML Pages</t>
-  </si>
-  <si>
     <t>NoSQL-DB Feedback</t>
   </si>
   <si>
@@ -155,28 +146,34 @@
     <t>SQL-Datenbank anlegen - DIZ</t>
   </si>
   <si>
-    <t>Testdaten erstellen - DIZ</t>
-  </si>
-  <si>
     <t>Webservice GET Bestellungen Kellner - LOT</t>
   </si>
   <si>
     <t>Webservice GET Bestellungen Koch - LOT</t>
   </si>
   <si>
-    <t>HTML Page für die Küche - MIK</t>
-  </si>
-  <si>
-    <t>Javascript Logik Küche - MIK</t>
-  </si>
-  <si>
-    <t>HTML Page für die Kellner - MIK</t>
-  </si>
-  <si>
-    <t>Javascript Logik Kellner - MIK</t>
-  </si>
-  <si>
     <t>Selectanweisungen Kellner,Koch - DIZ</t>
+  </si>
+  <si>
+    <t>Tabellen erstellen - DIZ</t>
+  </si>
+  <si>
+    <t>Tabellen Testdaten - DIZ</t>
+  </si>
+  <si>
+    <t>Webapp HTML&amp;JS Küche - MIK</t>
+  </si>
+  <si>
+    <t>Webapp HTML&amp;JS Kellner - MIK</t>
+  </si>
+  <si>
+    <t>GUI für die Android App - DIZ</t>
+  </si>
+  <si>
+    <t>Mockups HTML Pages - DIZ</t>
+  </si>
+  <si>
+    <t>Mockups Android App - DIZ</t>
   </si>
 </sst>
 </file>
@@ -269,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -304,6 +301,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -618,20 +616,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61EA23A4-825B-44B3-B87C-56BFEDE128BA}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="36.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -668,158 +664,150 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
+      <c r="A4" s="8" t="s">
+        <v>25</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>37</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
+      <c r="A5" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>36</v>
+        <v>33</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
+      <c r="A6" s="15" t="s">
+        <v>27</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="F6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
+      <c r="A7" t="s">
+        <v>29</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>27</v>
+      <c r="A8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>26</v>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>25</v>
+      <c r="D10" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F12" s="8" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="F12" s="12" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F15" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F16" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F17" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="F14" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>